<commit_message>
New CHA projects Fall 2022
</commit_message>
<xml_diff>
--- a/datasheets/All CHA Projects.xlsx
+++ b/datasheets/All CHA Projects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ststutzman\AppData\Local\Box\Box Edit\Documents\QVVXblqHz06eVgXeUUIHvw==\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinho\Documents\UIUC\OSF Academic Collaborations\Github\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_CDA61724C350D109D07E5E0318C8425FF2FD6879" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462851A9-E741-4122-94BD-D8A84D89C5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25065" windowHeight="11970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Projects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Closed Projects" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All Projects'!$A$1:$K$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All Projects'!$A$1:$K$18</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,6 +32,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="135">
   <si>
     <t>Project Number</t>
   </si>
@@ -74,6 +76,12 @@
     <t>Investigator 7</t>
   </si>
   <si>
+    <t>Investigator 8</t>
+  </si>
+  <si>
+    <t>Investigator 9</t>
+  </si>
+  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -270,6 +278,174 @@
   </si>
   <si>
     <t>https://app.box.com/folder/149697936703</t>
+  </si>
+  <si>
+    <t>C013</t>
+  </si>
+  <si>
+    <t>2022 Spring</t>
+  </si>
+  <si>
+    <t>Julie Traenkenschuh</t>
+  </si>
+  <si>
+    <t>Exploring Opportunities to Design and Implement Interventions to Increase Health Literacy in the African American, Medicaid Population</t>
+  </si>
+  <si>
+    <t>Brenikki Floyd</t>
+  </si>
+  <si>
+    <t>Kevin Garcia</t>
+  </si>
+  <si>
+    <t>C014</t>
+  </si>
+  <si>
+    <t>Telehealth to address health care disparities</t>
+  </si>
+  <si>
+    <t>Ananya Gangopadhyaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Radhika Sreedhar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yovia Xu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul Chastain</t>
+  </si>
+  <si>
+    <t>C016</t>
+  </si>
+  <si>
+    <t>Jacob Krive</t>
+  </si>
+  <si>
+    <t>Analytics and Artificial Intelligence for Cardio-Oncology</t>
+  </si>
+  <si>
+    <t>Chetan Bhardwaj, MD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Karl Kochendorfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravishankar Iyer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Christopher Gans</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Natalie Parde</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marianna Krive</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sandeep Kataria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Roopa Foulger</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arash Jalali</t>
+  </si>
+  <si>
+    <t>C017</t>
+  </si>
+  <si>
+    <t>Does providing free education on Medicare benefits improve health outcomes in working class communities?</t>
+  </si>
+  <si>
+    <t>Ben Shaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Uchechi Mitchell</t>
+  </si>
+  <si>
+    <t>C019</t>
+  </si>
+  <si>
+    <t>Using a community-based approach to improve health literacy and cancer screening rates in minority populations</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mary E. Stapel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stephen B. Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Michael G. Browne</t>
+  </si>
+  <si>
+    <t>C020</t>
+  </si>
+  <si>
+    <t>Ugo Buy</t>
+  </si>
+  <si>
+    <t>Pediatric Mental Health Model and Application Development in Connection with the School's Information Management System</t>
+  </si>
+  <si>
+    <t>Kyle W. Boerke</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sister M. Pieta Keller</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mark  Hallenbeck</t>
+  </si>
+  <si>
+    <t>C021</t>
+  </si>
+  <si>
+    <t>Jonathan Handler</t>
+  </si>
+  <si>
+    <t>Creating Human-Centered Decision Support Archetypes for CliniPane: a “Third Paradigm” in Clinical Decision Support</t>
+  </si>
+  <si>
+    <t>Kal Pasupathy</t>
+  </si>
+  <si>
+    <t>Elizabeth Lerner Papautsky</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Scott Barrows</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Spencer McDaniel</t>
+  </si>
+  <si>
+    <t>C022</t>
+  </si>
+  <si>
+    <t>Mansha Mirza</t>
+  </si>
+  <si>
+    <t>Telerehabilitation Disparities for Patients with Limited Proficiency</t>
+  </si>
+  <si>
+    <t>Courtney Pilat</t>
+  </si>
+  <si>
+    <t>C023</t>
+  </si>
+  <si>
+    <t>Pritikanta Paul</t>
+  </si>
+  <si>
+    <t>A text messaging based educational intervention aimed at improving outcomes in myasthenia gravis</t>
+  </si>
+  <si>
+    <t>Jorge Kattah</t>
+  </si>
+  <si>
+    <t>Biswajit Maharathi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dilip Pandey</t>
   </si>
 </sst>
 </file>
@@ -277,9 +453,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,12 +464,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA6A6A6"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -304,7 +491,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -312,12 +499,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -326,14 +565,40 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
@@ -342,9 +607,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -363,44 +625,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{85725FD2-6CE7-42C9-8CCC-3E4AC7D4C014}" name="Table3" displayName="Table3" ref="A1:N9" totalsRowShown="0">
-  <autoFilter ref="A1:N9" xr:uid="{85725FD2-6CE7-42C9-8CCC-3E4AC7D4C014}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{94D1B1C4-DB0B-4E1E-AE37-FB612EB8C22D}" name="Project Number"/>
-    <tableColumn id="2" xr3:uid="{51E7AB76-6A66-472C-8BBB-E2ACE54B2733}" name="RFP"/>
-    <tableColumn id="3" xr3:uid="{F3140DA2-6FE1-4B07-9E94-D77AFCC4E666}" name="PI"/>
-    <tableColumn id="4" xr3:uid="{33E510B9-02F1-41E4-96A4-3A55E4F5DF51}" name="Project Title" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{F25A5690-763E-451D-8B4F-2262864AF49E}" name="Investigator 1"/>
-    <tableColumn id="6" xr3:uid="{2BEE83E2-050B-42AE-92F3-5CF7C7D654F7}" name="Investigator 2"/>
-    <tableColumn id="7" xr3:uid="{79E16B86-F4FD-4A9F-B0EF-46B330F88D14}" name="Investigator 3"/>
-    <tableColumn id="8" xr3:uid="{832C98A6-F59A-4C2E-9637-9C52D83F38D4}" name="Investigator 4"/>
-    <tableColumn id="9" xr3:uid="{2E33E311-67F2-4918-84A6-9D9D82D352F3}" name="Investigator 5"/>
-    <tableColumn id="10" xr3:uid="{21FA5BC3-DB29-4688-8CE8-33970E39E61C}" name="Investigator 6"/>
-    <tableColumn id="11" xr3:uid="{8F9AA387-EC9F-4332-93D9-B24117A5722A}" name="Investigator 7"/>
-    <tableColumn id="13" xr3:uid="{F5FBBE19-5FF8-4277-8B48-A333E39BEDDA}" name="Amount" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{50F4A900-5D32-42C0-9C4E-048A075047AA}" name="Close Date" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{DFD33EED-81CD-4F43-AAC2-94D37DD31AA5}" name="Link"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:P18" totalsRowShown="0">
+  <autoFilter ref="A1:P18" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Project Number"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="RFP"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PI"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Project Title" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Investigator 1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Investigator 2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Investigator 3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Investigator 4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Investigator 5"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Investigator 6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Investigator 7"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Investigator 8"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Investigator 9"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Amount" totalsRowDxfId="0" dataCellStyle="Currency"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Close Date" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Link"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{961D79D1-B085-4392-A34D-07ED0A10B464}" name="Table2" displayName="Table2" ref="A1:L8" totalsRowShown="0">
-  <autoFilter ref="A1:L8" xr:uid="{961D79D1-B085-4392-A34D-07ED0A10B464}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:L8" totalsRowShown="0">
+  <autoFilter ref="A1:L8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{AB2EA566-B877-4C61-B2F6-A5AC971F93E5}" name="Project Number"/>
-    <tableColumn id="2" xr3:uid="{3C5E597D-68D6-4AFA-BD6D-4DA8765B885C}" name="RFP"/>
-    <tableColumn id="3" xr3:uid="{68AFEBE8-5795-4D18-9652-3BD597755A94}" name="PI"/>
-    <tableColumn id="4" xr3:uid="{AF6CCFE7-0309-4434-87B1-3C3DE13BBA68}" name="Project Title" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{6DD102ED-EF5A-4093-9A30-002AA116ADBF}" name="Investigator 1"/>
-    <tableColumn id="6" xr3:uid="{DCF48937-8FA2-446D-9990-C7D7B3F61158}" name="Investigator 2"/>
-    <tableColumn id="7" xr3:uid="{416A131D-FE82-4B0B-9F23-ECB127473106}" name="Investigator 3"/>
-    <tableColumn id="8" xr3:uid="{9F9C8DEC-2396-4D43-981C-AF8FB57B19FC}" name="Investigator 4"/>
-    <tableColumn id="9" xr3:uid="{6C85366D-F2B4-4594-81CD-BBE06054238D}" name="Investigator 5"/>
-    <tableColumn id="10" xr3:uid="{15AEB663-D720-4121-BC14-62B02805A3CA}" name="Investigator 6"/>
-    <tableColumn id="11" xr3:uid="{92ABAB5B-8130-49DF-AAA2-41DA91978F82}" name="Investigator 7"/>
-    <tableColumn id="12" xr3:uid="{546B9541-1586-4A99-A87C-DF340AE120EC}" name="Close Date" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Project Number"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="RFP"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="PI"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Project Title" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Investigator 1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Investigator 2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Investigator 3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Investigator 4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Investigator 5"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Investigator 6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Investigator 7"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Close Date" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -669,29 +933,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:P110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="15.88671875" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -734,285 +998,850 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="12">
+        <v>87882</v>
+      </c>
+      <c r="O2" s="2">
+        <v>44440</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="4">
-        <v>87882</v>
-      </c>
-      <c r="M2" s="2">
-        <v>44440</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="30">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
       <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="4">
+        <v>28</v>
+      </c>
+      <c r="N3" s="12">
         <v>194469</v>
       </c>
-      <c r="M3" s="2">
+      <c r="O3" s="2">
         <v>44909</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="30">
+      <c r="P3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="4">
+        <v>37</v>
+      </c>
+      <c r="N4" s="12">
         <v>105401</v>
       </c>
-      <c r="M4" s="2">
+      <c r="O4" s="2">
         <v>44865</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="P4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" s="12">
+        <v>39932</v>
+      </c>
+      <c r="O5" s="2">
+        <v>44896</v>
+      </c>
+      <c r="P5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="12">
+        <v>47563.399999999994</v>
+      </c>
+      <c r="O6" s="2">
+        <v>45078</v>
+      </c>
+      <c r="P6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="12">
+        <v>75000</v>
+      </c>
+      <c r="O7" s="2">
+        <v>44986</v>
+      </c>
+      <c r="P7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+      <c r="N8" s="12">
+        <v>73757</v>
+      </c>
+      <c r="O8" s="2">
+        <v>44986</v>
+      </c>
+      <c r="P8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N9" s="12">
+        <v>75009</v>
+      </c>
+      <c r="O9" s="2">
+        <v>44986</v>
+      </c>
+      <c r="P9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+      <c r="N10" s="12">
+        <v>74924.399999999994</v>
+      </c>
+      <c r="O10" s="2">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" t="s">
         <v>41</v>
       </c>
-      <c r="F5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5" s="4">
-        <v>39932</v>
-      </c>
-      <c r="M5" s="2">
-        <v>44896</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6" s="4">
-        <v>47563.399999999994</v>
-      </c>
-      <c r="M6" s="2">
+      <c r="F11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" t="s">
+        <v>90</v>
+      </c>
+      <c r="N11" s="12">
+        <v>69680</v>
+      </c>
+      <c r="O11" s="2">
         <v>45078</v>
       </c>
-      <c r="N6" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="30">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L7" s="4">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M12" t="s">
+        <v>102</v>
+      </c>
+      <c r="N12" s="12">
         <v>75000</v>
       </c>
-      <c r="M7" s="2">
-        <v>44986</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" t="s">
-        <v>64</v>
-      </c>
-      <c r="L8" s="4">
-        <v>73757</v>
-      </c>
-      <c r="M8" s="2">
-        <v>44986</v>
-      </c>
-      <c r="N8" s="5" t="s">
+      <c r="O12" s="2">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" t="s">
+        <v>106</v>
+      </c>
+      <c r="N13" s="12">
+        <v>74882</v>
+      </c>
+      <c r="O13" s="2">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="30">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" t="s">
-        <v>73</v>
-      </c>
-      <c r="J9" t="s">
-        <v>74</v>
-      </c>
-      <c r="K9" t="s">
-        <v>75</v>
-      </c>
-      <c r="L9" s="4">
-        <v>75009</v>
-      </c>
-      <c r="M9" s="2">
-        <v>44986</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>76</v>
-      </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" t="s">
+        <v>111</v>
+      </c>
+      <c r="N14" s="12">
+        <v>62136</v>
+      </c>
+      <c r="O14" s="2">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" t="s">
+        <v>117</v>
+      </c>
+      <c r="N15" s="12">
+        <v>74591</v>
+      </c>
+      <c r="O15" s="2">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" t="s">
+        <v>101</v>
+      </c>
+      <c r="N16" s="12">
+        <v>74891</v>
+      </c>
+      <c r="O16" s="2">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" t="s">
+        <v>128</v>
+      </c>
+      <c r="N17" s="12">
+        <v>74056</v>
+      </c>
+      <c r="O17" s="2">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" t="s">
+        <v>133</v>
+      </c>
+      <c r="G18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N18" s="12">
+        <v>74281</v>
+      </c>
+      <c r="O18" s="2">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="11"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="11"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E38" s="11"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E40" s="11"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E44" s="11"/>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E57" s="11"/>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E59" s="6"/>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E60" s="6"/>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E62" s="6"/>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E66" s="11"/>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E69" s="6"/>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E71" s="6"/>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E72" s="6"/>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E73" s="6"/>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E74" s="11"/>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E75" s="6"/>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E76" s="6"/>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E77" s="6"/>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E78" s="6"/>
+    </row>
+    <row r="79" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E79" s="7"/>
+    </row>
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E80" s="5"/>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E81" s="6"/>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E82" s="6"/>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E83" s="6"/>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E84" s="11"/>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E85" s="6"/>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E86" s="6"/>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E87" s="6"/>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E88" s="6"/>
+    </row>
+    <row r="89" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E89" s="7"/>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E90" s="5"/>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E91" s="6"/>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E92" s="6"/>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E93" s="6"/>
+    </row>
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E94" s="6"/>
+    </row>
+    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E95" s="11"/>
+    </row>
+    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E96" s="6"/>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E97" s="11"/>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E98" s="6"/>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E99" s="6"/>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E100" s="6"/>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E101" s="6"/>
+    </row>
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E102" s="11"/>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E103" s="6"/>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E104" s="6"/>
+    </row>
+    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E105" s="6"/>
+    </row>
+    <row r="106" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E106" s="7"/>
+    </row>
+    <row r="107" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E107" s="4"/>
+    </row>
+    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E108" s="5"/>
+    </row>
+    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E109" s="6"/>
+    </row>
+    <row r="110" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E110" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{8D0DA7CE-6792-4037-95F5-533577C68B61}"/>
-    <hyperlink ref="N3" r:id="rId2" xr:uid="{60E0B5E4-8253-403F-8D7F-71D83C65F7EE}"/>
-    <hyperlink ref="N4" r:id="rId3" xr:uid="{9647BC31-311B-4A6C-88CF-BC7C166340B4}"/>
-    <hyperlink ref="N6" r:id="rId4" xr:uid="{4F54BDD4-F901-4D9F-AD7F-35499036E1F2}"/>
-    <hyperlink ref="N5" r:id="rId5" xr:uid="{F5DD2AD7-2D55-4A45-A183-C899141B09AF}"/>
-    <hyperlink ref="N7" r:id="rId6" xr:uid="{4A5768EC-D729-4AA3-BB2C-4D4E99ED5391}"/>
-    <hyperlink ref="N8" r:id="rId7" xr:uid="{F7E6DE3F-5AE3-408C-893E-AD5C47F24D01}"/>
-    <hyperlink ref="N9" r:id="rId8" xr:uid="{68ACA07E-4277-4764-A018-0B9A21FECC1B}"/>
+    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="P3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="P4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="P6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="P5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="P7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="P8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="P9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
@@ -1023,29 +1852,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10485AA1-7AF2-49A8-988B-AB87525D91C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1080,204 +1909,204 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="45.75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L2" s="2">
         <v>44909</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30.75">
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L3" s="2">
         <v>44865</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L4" s="2">
         <v>44896</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L5" s="2">
         <v>45078</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30.75">
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L6" s="2">
         <v>44986</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30.75">
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L7" s="2">
         <v>44986</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="45.75">
+    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L8" s="2">
         <v>44986</v>
@@ -1292,19 +2121,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2778568-01F8-4DAB-9185-10B8E02886D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1339,24 +2168,24 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="30.75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L2" s="3">
         <v>44440</v>

</xml_diff>